<commit_message>
Start of Sunday 01/21
</commit_message>
<xml_diff>
--- a/ContentSheets/FLL_Website_Content_119.xlsx
+++ b/ContentSheets/FLL_Website_Content_119.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xgew1409\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah\Documents\GitHub\FFLSupport\ContentSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11670" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="17400" windowHeight="19530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="308">
   <si>
     <t xml:space="preserve">Category </t>
   </si>
@@ -957,12 +957,18 @@
   </si>
   <si>
     <t>Go4Zero</t>
+  </si>
+  <si>
+    <t>Static</t>
+  </si>
+  <si>
+    <t>Training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1003,7 +1009,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1022,6 +1028,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1036,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1082,6 +1100,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1363,7 +1393,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView topLeftCell="A48" workbookViewId="0">
@@ -3471,59 +3501,59 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B180"/>
+  <autoFilter ref="B1:B180" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" display="https://learning.aperianglobal.com/"/>
-    <hyperlink ref="D29" r:id="rId2"/>
-    <hyperlink ref="D17" r:id="rId3"/>
-    <hyperlink ref="D46" r:id="rId4"/>
-    <hyperlink ref="D49" r:id="rId5"/>
-    <hyperlink ref="D11" r:id="rId6"/>
-    <hyperlink ref="D39" r:id="rId7"/>
-    <hyperlink ref="D19" r:id="rId8"/>
-    <hyperlink ref="D7" r:id="rId9"/>
-    <hyperlink ref="D8" r:id="rId10"/>
-    <hyperlink ref="D15" r:id="rId11"/>
-    <hyperlink ref="D16" r:id="rId12"/>
-    <hyperlink ref="D30" r:id="rId13"/>
-    <hyperlink ref="D23" r:id="rId14"/>
-    <hyperlink ref="D14" r:id="rId15"/>
-    <hyperlink ref="D22" r:id="rId16"/>
-    <hyperlink ref="D50" r:id="rId17"/>
-    <hyperlink ref="D51" r:id="rId18"/>
-    <hyperlink ref="D52" r:id="rId19"/>
-    <hyperlink ref="D53" r:id="rId20"/>
-    <hyperlink ref="D54" r:id="rId21"/>
-    <hyperlink ref="D55" r:id="rId22"/>
-    <hyperlink ref="D56" r:id="rId23"/>
-    <hyperlink ref="D66" r:id="rId24"/>
-    <hyperlink ref="D67" r:id="rId25"/>
-    <hyperlink ref="D68" r:id="rId26"/>
-    <hyperlink ref="D70" r:id="rId27"/>
-    <hyperlink ref="D71" r:id="rId28"/>
-    <hyperlink ref="D72" r:id="rId29"/>
-    <hyperlink ref="D75" r:id="rId30"/>
-    <hyperlink ref="D42" r:id="rId31"/>
-    <hyperlink ref="D41" r:id="rId32"/>
-    <hyperlink ref="D43" r:id="rId33"/>
-    <hyperlink ref="D40" r:id="rId34"/>
-    <hyperlink ref="D44" r:id="rId35"/>
-    <hyperlink ref="D45" r:id="rId36"/>
-    <hyperlink ref="D37" r:id="rId37"/>
-    <hyperlink ref="D33" r:id="rId38"/>
-    <hyperlink ref="D32" r:id="rId39"/>
-    <hyperlink ref="D81" r:id="rId40"/>
-    <hyperlink ref="D34" r:id="rId41"/>
-    <hyperlink ref="D35" r:id="rId42"/>
-    <hyperlink ref="D36" r:id="rId43"/>
-    <hyperlink ref="D65" r:id="rId44"/>
-    <hyperlink ref="D87" r:id="rId45"/>
-    <hyperlink ref="D86" r:id="rId46"/>
-    <hyperlink ref="D85" r:id="rId47"/>
-    <hyperlink ref="D84" r:id="rId48"/>
-    <hyperlink ref="D83" r:id="rId49"/>
-    <hyperlink ref="D88" r:id="rId50"/>
-    <hyperlink ref="D148" r:id="rId51"/>
+    <hyperlink ref="D12" r:id="rId1" display="https://learning.aperianglobal.com/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D46" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D49" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D39" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D19" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D30" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D22" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D50" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D51" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D52" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D53" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D54" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D55" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D56" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="D66" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="D67" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="D68" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D70" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="D71" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D72" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D75" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="D42" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D41" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="D43" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D40" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="D44" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="D45" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="D37" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="D33" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="D32" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="D81" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="D34" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="D35" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="D36" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="D65" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D87" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="D86" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="D85" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="D84" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="D83" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="D88" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="D148" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId52"/>
@@ -3531,7 +3561,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3681,20 +3711,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
-    <hyperlink ref="B9" r:id="rId4"/>
-    <hyperlink ref="B12" r:id="rId5"/>
-    <hyperlink ref="B14" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -3887,19 +3918,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://learning.aperianglobal.com/"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://learning.aperianglobal.com/" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -4026,14 +4058,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -4168,32 +4201,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B7" r:id="rId5"/>
-    <hyperlink ref="B8" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B10" r:id="rId8"/>
-    <hyperlink ref="B11" r:id="rId9"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="77.42578125" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -4204,182 +4238,193 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>39</v>
-      </c>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="20" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>32</v>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="11">
+        <v>77487</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B14" s="11">
+        <v>77493</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="B15" s="21">
+        <v>80504</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B16" s="11">
         <v>78983</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B17" s="11">
         <v>78984</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B14" s="11">
-        <v>78975</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B15" s="11">
-        <v>78960</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="B18" s="11">
+        <v>78975</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>172</v>
+        <v>153</v>
+      </c>
+      <c r="B19" s="11">
+        <v>78960</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4482,16 +4527,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4513,11 +4559,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4548,11 +4595,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -4794,18 +4842,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
@@ -4897,19 +4946,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -5112,19 +5162,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B9" r:id="rId6"/>
-    <hyperlink ref="B10" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B17" r:id="rId9"/>
-    <hyperlink ref="B19" r:id="rId10"/>
-    <hyperlink ref="B20" r:id="rId11"/>
-    <hyperlink ref="B21" r:id="rId12"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="B19" r:id="rId10" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="B20" r:id="rId11" xr:uid="{00000000-0004-0000-0800-00000A000000}"/>
+    <hyperlink ref="B21" r:id="rId12" xr:uid="{00000000-0004-0000-0800-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>